<commit_message>
Mom, i'm in trixyu!
</commit_message>
<xml_diff>
--- a/source/test.xlsx
+++ b/source/test.xlsx
@@ -1,87 +1,93 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\node_xlsx_parser\source\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
   </bookViews>
   <sheets>
-    <sheet name="Механика" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Механика" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="OLE_LINK1" localSheetId="0">Механика!#REF!</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
-  <si>
-    <t xml:space="preserve">Механические явления</t>
-  </si>
-  <si>
-    <t xml:space="preserve">№ теста</t>
-  </si>
-  <si>
-    <t xml:space="preserve">№ п/п</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вид задания</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТЕМА Задания</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Опциональный комментарий к заданию</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Код вида задания</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Описание вида задания</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Комментарий для программистов</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Критичность задания</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Аналог задания из финального теста</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Текст вопроса (рисунок)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="81">
+  <si>
+    <t>Механические явления</t>
+  </si>
+  <si>
+    <t>№ теста</t>
+  </si>
+  <si>
+    <t>№ п/п</t>
+  </si>
+  <si>
+    <t>Вид задания</t>
+  </si>
+  <si>
+    <t>ТЕМА Задания</t>
+  </si>
+  <si>
+    <t>Опциональный комментарий к заданию</t>
+  </si>
+  <si>
+    <t>Код вида задания</t>
+  </si>
+  <si>
+    <t>Описание вида задания</t>
+  </si>
+  <si>
+    <t>Комментарий для программистов</t>
+  </si>
+  <si>
+    <t>Критичность задания</t>
+  </si>
+  <si>
+    <t>Аналог задания из финального теста</t>
+  </si>
+  <si>
+    <t>Текст вопроса (рисунок)</t>
   </si>
   <si>
     <t xml:space="preserve">Задание 1 </t>
   </si>
   <si>
-    <t xml:space="preserve">Ответ 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задание 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ответ 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задание 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ответ 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задание 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ответ 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задание 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ответ 5</t>
+    <t>Ответ 1</t>
+  </si>
+  <si>
+    <t>Задание 2</t>
+  </si>
+  <si>
+    <t>Ответ 2</t>
+  </si>
+  <si>
+    <t>Задание 3</t>
+  </si>
+  <si>
+    <t>Ответ 3</t>
+  </si>
+  <si>
+    <t>Задание 4</t>
+  </si>
+  <si>
+    <t>Ответ 4</t>
+  </si>
+  <si>
+    <t>Задание 5</t>
+  </si>
+  <si>
+    <t>Ответ 5</t>
   </si>
   <si>
     <t>000005</t>
@@ -90,31 +96,31 @@
     <t>one_option</t>
   </si>
   <si>
-    <t xml:space="preserve">Свободное падение тел</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Задание базового уровня</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001 (5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5 вариантов вопроса, 1 из 5 правильный ответ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Есть ли возможность вынести такие задания в отдельный код? От 2 до 5 вариаций. Как тут, например, в 1 задании - 5 на 5, во втором - 3 на 3.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Соотнесите формулу с измеряемой величиной</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Проекция начальной скорости</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Проекция мгновенной скорости</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Проекция перемещения</t>
+    <t>Свободное падение тел</t>
+  </si>
+  <si>
+    <t>Задание базового уровня</t>
+  </si>
+  <si>
+    <t>001 (5)</t>
+  </si>
+  <si>
+    <t>5 вариантов вопроса, 1 из 5 правильный ответ</t>
+  </si>
+  <si>
+    <t>Есть ли возможность вынести такие задания в отдельный код? От 2 до 5 вариаций. Как тут, например, в 1 задании - 5 на 5, во втором - 3 на 3.</t>
+  </si>
+  <si>
+    <t>Соотнесите формулу с измеряемой величиной</t>
+  </si>
+  <si>
+    <t>Проекция начальной скорости</t>
+  </si>
+  <si>
+    <t>Проекция мгновенной скорости</t>
+  </si>
+  <si>
+    <t>Проекция перемещения</t>
   </si>
   <si>
     <t>Время</t>
@@ -123,64 +129,64 @@
     <t>Координата</t>
   </si>
   <si>
-    <t xml:space="preserve">001 (3)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3 варианта вопроса, 1 из 3 правильный ответ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рубежный вопрос</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Дополните предложение</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Скорость тела, подброшенного вертикально вверх</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Постепенно уменьшается</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Скорость тела, падающего вертикально вниз</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Постепенно увеличивается</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Горизонтальная проекция скорости тела, подброшенного вверх</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Не изменяется</t>
+    <t>001 (3)</t>
+  </si>
+  <si>
+    <t>3 варианта вопроса, 1 из 3 правильный ответ</t>
+  </si>
+  <si>
+    <t>Рубежный вопрос</t>
+  </si>
+  <si>
+    <t>Дополните предложение</t>
+  </si>
+  <si>
+    <t>Скорость тела, подброшенного вертикально вверх</t>
+  </si>
+  <si>
+    <t>Постепенно уменьшается</t>
+  </si>
+  <si>
+    <t>Скорость тела, падающего вертикально вниз</t>
+  </si>
+  <si>
+    <t>Постепенно увеличивается</t>
+  </si>
+  <si>
+    <t>Горизонтальная проекция скорости тела, подброшенного вверх</t>
+  </si>
+  <si>
+    <t>Не изменяется</t>
   </si>
   <si>
     <t>002</t>
   </si>
   <si>
-    <t xml:space="preserve">1 варианнт вопроса, только 1 из 5 вариантов ответа - правильный</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Договорились всегда помещать правильный ответ в графу Ответ 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Причиной свободного падения тел является</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Правильный ответ ---&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Сила тяжести</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ускорение свободного падения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Центростремительнос ускорение при вращении земли</t>
+    <t>1 варианнт вопроса, только 1 из 5 вариантов ответа - правильный</t>
+  </si>
+  <si>
+    <t>Договорились всегда помещать правильный ответ в графу Ответ 1</t>
+  </si>
+  <si>
+    <t>Причиной свободного падения тел является</t>
+  </si>
+  <si>
+    <t>Правильный ответ ---&gt;</t>
+  </si>
+  <si>
+    <t>Сила тяжести</t>
+  </si>
+  <si>
+    <t>Ускорение свободного падения</t>
+  </si>
+  <si>
+    <t>Центростремительнос ускорение при вращении земли</t>
   </si>
   <si>
     <t>Масса</t>
   </si>
   <si>
-    <t xml:space="preserve">Давление со стороны атмосферы</t>
+    <t>Давление со стороны атмосферы</t>
   </si>
   <si>
     <t>many_option</t>
@@ -189,126 +195,120 @@
     <t>003</t>
   </si>
   <si>
-    <t xml:space="preserve">Можно выбрать от 1 до 5 вариантов одновременно</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Если вариант ответа из графы "Ответ N"  является правильным - в графе "Задание N" будет знак (1 или +)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Свободно падающим является тело:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Камень, скатившийся с края обрыва</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Птица в полёте</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Леопард, отдыхающий на пальме</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Снаряд, вылетивший из пушки</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Все перечисленные варианты</t>
+    <t>Можно выбрать от 1 до 5 вариантов одновременно</t>
+  </si>
+  <si>
+    <t>Если вариант ответа из графы "Ответ N"  является правильным - в графе "Задание N" будет знак (1 или +)</t>
+  </si>
+  <si>
+    <t>Свободно падающим является тело:</t>
+  </si>
+  <si>
+    <t>Камень, скатившийся с края обрыва</t>
+  </si>
+  <si>
+    <t>Птица в полёте</t>
+  </si>
+  <si>
+    <t>Леопард, отдыхающий на пальме</t>
+  </si>
+  <si>
+    <t>Снаряд, вылетивший из пушки</t>
+  </si>
+  <si>
+    <t>Все перечисленные варианты</t>
   </si>
   <si>
     <t>004</t>
   </si>
   <si>
-    <t xml:space="preserve">Расположить элементы в верной пследовательности</t>
-  </si>
-  <si>
-    <t xml:space="preserve">В колонках "задание N" будут последовательности, в колонках "ответ N" - верный вариант последовательности. В принципе, алгоритм аналогичен коду задания 001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Выберите верные утверждения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Движение тела, брошенного вертикально вверх - частный случай свободного падения; 2) Максимальная скорость приобретается телом в верхней точке; 3) Свободному падению подвержены только тяжелые тела; 4) время подъёма тела при н.у. равно времени падения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) 1,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1) Движение тела, брошенного вертикально вверх не является свободным падением; 2) Максимальная скорость приобретается телом в нижней точке; 3)  время подъёма тела при н.у. меньше времени падения; 4) Свободному падению подвержены любые тела</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2) 2,4</t>
+    <t>Расположить элементы в верной пследовательности</t>
+  </si>
+  <si>
+    <t>В колонках "задание N" будут последовательности, в колонках "ответ N" - верный вариант последовательности. В принципе, алгоритм аналогичен коду задания 001</t>
+  </si>
+  <si>
+    <t>Выберите верные утверждения</t>
+  </si>
+  <si>
+    <t>1) Движение тела, брошенного вертикально вверх - частный случай свободного падения; 2) Максимальная скорость приобретается телом в верхней точке; 3) Свободному падению подвержены только тяжелые тела; 4) время подъёма тела при н.у. равно времени падения</t>
+  </si>
+  <si>
+    <t>1) 1,4</t>
+  </si>
+  <si>
+    <t>1) Движение тела, брошенного вертикально вверх не является свободным падением; 2) Максимальная скорость приобретается телом в нижней точке; 3)  время подъёма тела при н.у. меньше времени падения; 4) Свободному падению подвержены любые тела</t>
+  </si>
+  <si>
+    <t>2) 2,4</t>
   </si>
   <si>
     <t xml:space="preserve">1)  Свободному падению подвержены только тяжелые тела;  2) время подъёма тела при н.у. равно времени падения 3) Движение тела, брошенного вертикально вверх - частный случай свободного падения; 4) Максимальная скорость приобретается телом в верхней точке; </t>
   </si>
   <si>
-    <t xml:space="preserve">3) 2,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Максимальная скорость приобретается телом в нижней точке; 2) Движение тела, брошенного вертикально вверх не является свободным падением;  3) Свободному падению подвержены любые тела; 4) время подъёма тела при н.у. меньше времени падения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4) 1,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1)Максимальная скорость приобретается телом в нижней точке; 2) Движение тела, брошенного вертикально вверх является частным случаем свободного падения;  3) Свободному падению подвержены только тела легче воздуха; 4) время подъёма тела при н.у.больше времени падения</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5) 1,2</t>
+    <t>3) 2,3</t>
+  </si>
+  <si>
+    <t>1)Максимальная скорость приобретается телом в нижней точке; 2) Движение тела, брошенного вертикально вверх не является свободным падением;  3) Свободному падению подвержены любые тела; 4) время подъёма тела при н.у. меньше времени падения</t>
+  </si>
+  <si>
+    <t>4) 1,3</t>
+  </si>
+  <si>
+    <t>1)Максимальная скорость приобретается телом в нижней точке; 2) Движение тела, брошенного вертикально вверх является частным случаем свободного падения;  3) Свободному падению подвержены только тела легче воздуха; 4) время подъёма тела при н.у.больше времени падения</t>
+  </si>
+  <si>
+    <t>5) 1,2</t>
+  </si>
+  <si>
+    <t>one_option_many_question</t>
+  </si>
+  <si>
+    <t>correct_option_sequence</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
     </font>
     <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color theme="10"/>
-      <sz val="11.000000"/>
-      <u/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <color theme="11"/>
-      <sz val="11.000000"/>
-      <u/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <b/>
+      <sz val="11"/>
       <color indexed="64"/>
-      <sz val="12.000000"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <b/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="9"/>
       <color indexed="64"/>
-      <sz val="11.000000"/>
+      <name val="Verdana"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <i/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
-    </font>
-    <font>
-      <name val="Verdana"/>
-      <color indexed="64"/>
-      <sz val="9.000000"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <color indexed="64"/>
-      <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -400,185 +400,153 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="7" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="41">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="3" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="4" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="5" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="6" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="7" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="8" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="9" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="10" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="11" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="12" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="13" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="14" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="15" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="16" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="17" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="18" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="19" builtinId="8"/>
-    <cellStyle name="Гиперссылка" xfId="20" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="21" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="22" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="23" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="24" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="25" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="26" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="27" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="28" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="29" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="30" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="31" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="32" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="33" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="34" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="35" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="36" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="37" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="38" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="39" builtinId="9"/>
-    <cellStyle name="Открывавшаяся гиперссылка" xfId="40" builtinId="9"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
@@ -592,11 +560,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="AutoShape 5" descr="https://fs.znanio.ru/methodology/images/47/69/47699756121fcddae4693c2e74f5871a5ea9c67f.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 5" descr="https://fs.znanio.ru/methodology/images/47/69/47699756121fcddae4693c2e74f5871a5ea9c67f.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -625,11 +593,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7170" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7170" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -658,11 +626,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7171" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7171" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -691,11 +659,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7172" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7172" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -724,11 +692,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7173" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7173" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -757,11 +725,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7176" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7176" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -790,11 +758,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7177" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7177" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -823,11 +791,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7179" name="AutoShape 11" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7179" name="AutoShape 11" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -856,11 +824,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7180" name="AutoShape 12" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7180" name="AutoShape 12" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -889,11 +857,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7183" name="AutoShape 15" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7183" name="AutoShape 15" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -922,11 +890,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7184" name="AutoShape 16" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7184" name="AutoShape 16" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -955,11 +923,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7185" name="AutoShape 17" descr="https://ds05.infourok.ru/uploads/ex/1132/00098711-c9ce47f6/hello_html_m58451734.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7185" name="AutoShape 17" descr="https://ds05.infourok.ru/uploads/ex/1132/00098711-c9ce47f6/hello_html_m58451734.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -988,11 +956,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7186" name="AutoShape 18" descr="https://ds05.infourok.ru/uploads/ex/0640/00124237-d2b09fb7/img1.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7186" name="AutoShape 18" descr="https://ds05.infourok.ru/uploads/ex/0640/00124237-d2b09fb7/img1.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1021,11 +989,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7188" name="AutoShape 20" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7188" name="AutoShape 20" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1054,11 +1022,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7189" name="AutoShape 21" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7189" name="AutoShape 21" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1087,11 +1055,11 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7190" name="AutoShape 22" descr="https://fsd.kopilkaurokov.ru/up/html/2019/12/22/k_5dffb8c40bb25/user_file_5dffb8c5c53a5_0_1.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7190" name="AutoShape 22" descr="https://fsd.kopilkaurokov.ru/up/html/2019/12/22/k_5dffb8c40bb25/user_file_5dffb8c5c53a5_0_1.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1120,11 +1088,11 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="AutoShape 5" descr="https://fs.znanio.ru/methodology/images/47/69/47699756121fcddae4693c2e74f5871a5ea9c67f.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="AutoShape 5" descr="https://fs.znanio.ru/methodology/images/47/69/47699756121fcddae4693c2e74f5871a5ea9c67f.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1153,11 +1121,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1186,11 +1154,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1219,11 +1187,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1252,11 +1220,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1285,11 +1253,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1318,11 +1286,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1351,11 +1319,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="60" name="AutoShape 11" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="AutoShape 11" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1384,11 +1352,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="AutoShape 12" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="AutoShape 12" descr="https://i.pinimg.com/originals/83/15/d7/8315d7bff2f3c9cfd4aa67f551f7009b.gif"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1417,11 +1385,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="AutoShape 15" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="AutoShape 15" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1450,11 +1418,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="63" name="AutoShape 16" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="AutoShape 16" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1483,11 +1451,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="64" name="AutoShape 17" descr="https://ds05.infourok.ru/uploads/ex/1132/00098711-c9ce47f6/hello_html_m58451734.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="AutoShape 17" descr="https://ds05.infourok.ru/uploads/ex/1132/00098711-c9ce47f6/hello_html_m58451734.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1516,11 +1484,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="65" name="AutoShape 18" descr="https://ds05.infourok.ru/uploads/ex/0640/00124237-d2b09fb7/img1.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="AutoShape 18" descr="https://ds05.infourok.ru/uploads/ex/0640/00124237-d2b09fb7/img1.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1549,11 +1517,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="66" name="AutoShape 19" descr="https://ds05.infourok.ru/uploads/ex/0640/00124237-d2b09fb7/img1.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="AutoShape 19" descr="https://ds05.infourok.ru/uploads/ex/0640/00124237-d2b09fb7/img1.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1582,11 +1550,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="AutoShape 20" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="AutoShape 20" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1615,11 +1583,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="68" name="AutoShape 21" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="AutoShape 21" descr="https://d.120-bal.ru/pars_docs/refs/27/26709/26709_html_m1b940305.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1648,11 +1616,11 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="69" name="AutoShape 22" descr="https://fsd.kopilkaurokov.ru/up/html/2019/12/22/k_5dffb8c40bb25/user_file_5dffb8c5c53a5_0_1.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="AutoShape 22" descr="https://fsd.kopilkaurokov.ru/up/html/2019/12/22/k_5dffb8c40bb25/user_file_5dffb8c5c53a5_0_1.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1681,11 +1649,11 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="96" name="AutoShape 11" descr="https://ds05.infourok.ru/uploads/ex/078d/000b65b4-4199be5a/hello_html_m720fbf96.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="AutoShape 11" descr="https://ds05.infourok.ru/uploads/ex/078d/000b65b4-4199be5a/hello_html_m720fbf96.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1714,11 +1682,11 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="97" name="AutoShape 12" descr="https://ds05.infourok.ru/uploads/ex/078d/000b65b4-4199be5a/hello_html_m720fbf96.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="AutoShape 12" descr="https://ds05.infourok.ru/uploads/ex/078d/000b65b4-4199be5a/hello_html_m720fbf96.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1749,13 +1717,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-59-30.jpg" hidden="0"/>
+        <xdr:cNvPr id="1025" name="Picture 1" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-59-30.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -1786,13 +1754,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1026" name="Picture 2" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-58-28.jpg" hidden="0"/>
+        <xdr:cNvPr id="1026" name="Picture 2" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-58-28.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -1823,13 +1791,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1027" name="Picture 3" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-59-18.jpg" hidden="0"/>
+        <xdr:cNvPr id="1027" name="Picture 3" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-59-18.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -1860,13 +1828,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1028" name="Picture 4" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-58-53.jpg" hidden="0"/>
+        <xdr:cNvPr id="1028" name="Picture 4" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-58-53.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -1897,13 +1865,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1029" name="Picture 5" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-58-42.jpg" hidden="0"/>
+        <xdr:cNvPr id="1029" name="Picture 5" descr="https://uchitel.pro/wp-content/uploads/2018/10/2018-10-09_21-58-42.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
@@ -1932,11 +1900,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1965,11 +1933,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="78" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -1998,11 +1966,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="79" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2031,11 +1999,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="80" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2064,11 +2032,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="81" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2097,11 +2065,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="82" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="82" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2130,11 +2098,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="83" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="83" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2163,11 +2131,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="84" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="84" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2196,11 +2164,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="85" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2229,11 +2197,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="86" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2262,11 +2230,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="87" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="87" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2295,11 +2263,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="88" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="88" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2328,11 +2296,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="89" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="89" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2361,11 +2329,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="90" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="90" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2394,11 +2362,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="91" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="91" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2427,11 +2395,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="92" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="92" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2460,11 +2428,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="AutoShape 4" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2493,11 +2461,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="94" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="94" name="AutoShape 2" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2526,11 +2494,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="95" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="95" name="AutoShape 3" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2559,11 +2527,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="98" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="98" name="AutoShape 5" descr="https://cf2.ppt-online.org/files2/slide/7/7jxzCNku86D2cXielZaGREAbytKpO5PLnB4doS/slide-6.jpg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2592,11 +2560,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="99" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="99" name="AutoShape 8" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2625,11 +2593,11 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="100" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png" hidden="0"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeArrowheads="1" noChangeAspect="1"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="100" name="AutoShape 9" descr="https://fs00.infourok.ru/images/doc/255/259794/hello_html_1cd9b881.png"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2648,291 +2616,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3135,46 +2820,48 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <outlinePr applyStyles="0" showOutlineSymbols="1" summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr autoPageBreaks="1" fitToPage="1"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A2:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="55">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="T12" activeCellId="0" sqref="T12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="T12" sqref="T12"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="4"/>
-    <col customWidth="1" min="3" max="3" width="15"/>
-    <col customWidth="1" min="4" max="4" width="22.28515625"/>
-    <col customWidth="1" min="5" max="5" width="20.140625"/>
-    <col customWidth="1" min="6" max="6" width="13"/>
-    <col customWidth="1" min="7" max="7" width="30.85546875"/>
-    <col customWidth="1" min="8" max="8" width="49.7109375"/>
-    <col customWidth="1" min="9" max="9" width="36.85546875"/>
-    <col customWidth="1" min="10" max="10" width="16.140625"/>
-    <col customWidth="1" min="11" max="11" width="38.42578125"/>
-    <col customWidth="1" min="12" max="12" width="39.5703125"/>
-    <col customWidth="1" min="13" max="13" width="27.28515625"/>
-    <col customWidth="1" min="14" max="14" width="37.85546875"/>
-    <col customWidth="1" min="15" max="15" width="27"/>
-    <col customWidth="1" min="16" max="16" width="36.7109375"/>
-    <col customWidth="1" min="17" max="17" width="25"/>
-    <col customWidth="1" min="18" max="18" width="33.85546875"/>
-    <col customWidth="1" min="19" max="19" width="25.140625"/>
-    <col customWidth="1" min="20" max="20" width="34.140625"/>
-    <col customWidth="1" min="21" max="21" width="25.7109375"/>
+    <col min="2" max="2" width="4" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="49.7109375" customWidth="1"/>
+    <col min="9" max="9" width="36.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="38.42578125" customWidth="1"/>
+    <col min="12" max="12" width="39.5703125" customWidth="1"/>
+    <col min="13" max="13" width="27.28515625" customWidth="1"/>
+    <col min="14" max="14" width="37.85546875" customWidth="1"/>
+    <col min="15" max="15" width="27" customWidth="1"/>
+    <col min="16" max="16" width="36.7109375" customWidth="1"/>
+    <col min="17" max="17" width="25" customWidth="1"/>
+    <col min="18" max="18" width="33.85546875" customWidth="1"/>
+    <col min="19" max="19" width="25.140625" customWidth="1"/>
+    <col min="20" max="20" width="34.140625" customWidth="1"/>
+    <col min="21" max="21" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -3182,7 +2869,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -3190,12 +2877,12 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" ht="16.5">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" ht="42.75">
+    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -3260,7 +2947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" ht="89.25" customHeight="1">
+    <row r="7" spans="1:21" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -3268,7 +2955,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>24</v>
@@ -3312,7 +2999,7 @@
       </c>
       <c r="U7" s="13"/>
     </row>
-    <row r="8" ht="66.75" customHeight="1">
+    <row r="8" spans="1:21" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
@@ -3320,7 +3007,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>24</v>
@@ -3340,7 +3027,9 @@
       <c r="I8" s="10">
         <v>1</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
       <c r="K8" s="10" t="s">
         <v>38</v>
       </c>
@@ -3367,7 +3056,7 @@
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
     </row>
-    <row r="9" ht="133.5" customHeight="1">
+    <row r="9" spans="1:21" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
@@ -3395,7 +3084,9 @@
       <c r="I9" s="10">
         <v>0</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
       <c r="K9" s="10" t="s">
         <v>48</v>
       </c>
@@ -3422,7 +3113,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" ht="174" customHeight="1">
+    <row r="10" spans="1:21" ht="174" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
@@ -3450,7 +3141,9 @@
       <c r="I10" s="10">
         <v>0</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
       <c r="K10" s="10" t="s">
         <v>59</v>
       </c>
@@ -3477,15 +3170,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" ht="138.75" customHeight="1">
+    <row r="11" spans="1:21" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="19">
         <v>5</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>23</v>
+      <c r="C11" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>24</v>
@@ -3505,7 +3198,9 @@
       <c r="I11" s="10">
         <v>0</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
       <c r="K11" s="9" t="s">
         <v>68</v>
       </c>
@@ -3540,72 +3235,72 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" ht="137.25" customHeight="1">
+    <row r="12" spans="1:21" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N12" s="17"/>
       <c r="O12" s="20"/>
       <c r="P12" s="21"/>
     </row>
-    <row r="13" ht="121.5" customHeight="1">
+    <row r="13" spans="1:21" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N13" s="22"/>
       <c r="O13" s="23"/>
       <c r="P13" s="22"/>
     </row>
-    <row r="14" ht="189.75" customHeight="1">
+    <row r="14" spans="1:21" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N14" s="18"/>
       <c r="O14" s="21"/>
       <c r="P14" s="18"/>
     </row>
-    <row r="15" ht="96" customHeight="1">
+    <row r="15" spans="1:21" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N15" s="18"/>
       <c r="O15" s="24"/>
       <c r="P15" s="17"/>
     </row>
-    <row r="16" ht="214.5" customHeight="1">
+    <row r="16" spans="1:21" ht="214.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N16" s="17"/>
       <c r="O16" s="25"/>
       <c r="P16" s="17"/>
     </row>
-    <row r="19">
+    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N19" s="25"/>
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
     </row>
-    <row r="20" ht="123" customHeight="1">
+    <row r="20" spans="14:16" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N20" s="17"/>
       <c r="O20" s="25"/>
       <c r="P20" s="25"/>
     </row>
-    <row r="21" ht="181.5" customHeight="1">
+    <row r="21" spans="14:16" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N21" s="17"/>
       <c r="O21" s="25"/>
       <c r="P21" s="25"/>
     </row>
-    <row r="22" ht="105" customHeight="1">
+    <row r="22" spans="14:16" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N22" s="26"/>
       <c r="O22" s="21"/>
       <c r="P22" s="27"/>
     </row>
-    <row r="23" ht="93" customHeight="1">
+    <row r="23" spans="14:16" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N23" s="21"/>
       <c r="O23" s="21"/>
       <c r="P23" s="18"/>
     </row>
-    <row r="24" ht="120.75" customHeight="1">
+    <row r="24" spans="14:16" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N24" s="18"/>
       <c r="O24" s="28"/>
       <c r="P24" s="18"/>
     </row>
-    <row r="25">
+    <row r="25" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N25" s="18"/>
       <c r="O25" s="28"/>
       <c r="P25" s="18"/>
     </row>
-    <row r="26">
+    <row r="26" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N26" s="17"/>
       <c r="O26" s="21"/>
       <c r="P26" s="17"/>
     </row>
-    <row r="27">
+    <row r="27" spans="14:16" x14ac:dyDescent="0.25">
       <c r="N27" s="17"/>
       <c r="O27" s="28"/>
       <c r="P27" s="17"/>
@@ -3614,80 +3309,20 @@
   <mergeCells count="1">
     <mergeCell ref="F2:K3"/>
   </mergeCells>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="landscape" pageOrder="downThenOver" paperSize="9" scale="22" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
-  <headerFooter/>
+  <conditionalFormatting sqref="M8 O8 Q8 S8 U8">
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U9 O9 Q9 S9">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11 O11 Q11 S11 U11">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12 J12 L12 N12 P12">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="9" scale="22" firstPageNumber="0" orientation="landscape"/>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="6" id="{009B00E0-0047-46A9-B064-002700B800B1}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>M8 O8 Q8 S8 U8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="4" id="{00F7005B-009D-4E00-9FAD-00200050003F}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>U9 O9 Q9 S9</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="2" id="{00EA0053-00F8-4D03-8B16-006B00040031}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>M11 O11 Q11 S11 U11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="duplicateValues" priority="1" id="{00CA0091-0030-4419-89AA-009C005D0095}">
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFFC7CE"/>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H12 J12 L12 N12 P12</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>